<commit_message>
nytt søkesystem og bugsixes
</commit_message>
<xml_diff>
--- a/Diku.xlsx
+++ b/Diku.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\OneDrive\Dokumenter\DIKU\DIKU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B345B420-A32E-442F-82D7-FBA72B9C59B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F71400-E054-4E62-80DB-CF6F8D1B72DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1047,9 +1047,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Studenten: har kunnskap om hvordan man identifiserer og analyserer utfordringer knyttet til prosjektets initieringsfase, og kan definere forutsetninger for prosjektsuksess, ​har grunnleggende kunnskap om avhengigheten mellom prosjekteiers forretningsmessige mål,  bygningsdesign, teknologibruk og støttefunksjoner og hvordan dette forstås i et helhetlig perspektiv, forstår prosjekteringsprosessen og dens plass i den samlede byggeprosessen, har kunnskap om produkt som brukes i  prosjekteringsprosess  og hva som utgjør verdi i dem, har kunnskap om kompleksiteten i  byggeprosjekter, behovet for tverrfaglig samarbeid og håndtering av grensesnitt, forstår viktigheten av profesjonell styring av prosjekteringsprosess for å gjøre prosjektet egnet for bruker og eiers formål, har inngående kunnskap om de vanligste tids- og kostnadsestimeringsmetodene, har inngående kunnskap om analysemetoder som livssyklus-,  kostnads- og interessentanalyse, kan beskrive hovedkategoriene av prosjektorganisasjonsstrukturer (prosjekt, klassisk og matrise), og forstår fordeler og ulemper ved de forskjellige modellene, har kunnskap om forskjellige kontrakts-  og prosjektleveringsmodeller, inkludert nye, innovative samarbeidsmodeller. </t>
-  </si>
-  <si>
     <t>Studenten: kan etablere riktige prosjektmål og suksesskriterier, forstår hensikten med Work Break Down Structure (WBS) og hvordan denne skal utarbeides, har kunnskap om hvilke verktøy som kan brukes i en usikkerhets- / risikostyringsprosess, kan løse utfordringer knyttet til økonomiske begrensninger i prosjektet ved hjelp av utjevning av ressurser, brukt tid, endring av relasjoner eller bruk av flyt / slakk, kan bruke indekser (for eksempel kostnads- og tidsindekser) for løpende å kunne overvåke prosjektstatus og for å etablere riktige prognoser, kan styre prosjekteringsprosessen.</t>
   </si>
   <si>
@@ -1857,6 +1854,9 @@
   </si>
   <si>
     <t>Læringsutbytte - Generell Kompetanse</t>
+  </si>
+  <si>
+    <t>Studenten: har kunnskap om hvordan man identifiserer og analyserer utfordringer knyttet til prosjektets initieringsfase, og kan definere forutsetninger for prosjektsuksess, har grunnleggende kunnskap om avhengigheten mellom prosjekteiers forretningsmessige mål, bygningsdesign, teknologibruk og støttefunksjoner og hvordan dette forstås i et helhetlig perspektiv, forstår prosjekteringsprosessen og dens plass i den samlede byggeprosessen, har kunnskap om produkt som brukes i prosjekteringsprosess og hva som utgjør verdi i dem, har kunnskap om kompleksitet i byggeprosjekter, behovet for tverrfaglig samarbeid og håndtering av grensesnitt, forstår viktigheten av profesjonell styring av prosjekteringsprosess for å gjøre prosjektet egnet for bruker og eiers formål, har inngående kunnskap om de vanligste tids- og kostnadsestimeringsmetodene, har inngående kunnskap om analysemetoder som livssyklus-, kostnads- og interessentanalyse, kan beskrive hovedkategoriene av prosjektorganisasjonsstrukturer (prosjekt, klassisk og matrise), og forstår fordeler og ulemper ved de forskjellige modellene, har kunnskap om forskjellige kontrakts- og prosjektleveringsmodeller, inkludert nye, innovative samarbeidsmodeller.</t>
   </si>
 </sst>
 </file>
@@ -3871,8 +3871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCDD31-3723-4F19-8F81-7049F051B343}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="K11" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3913,7 +3913,7 @@
         <v>182</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>183</v>
@@ -3946,7 +3946,7 @@
         <v>267</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="325.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4024,10 +4024,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="19" t="s">
+        <v>573</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>574</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>575</v>
       </c>
       <c r="K3" s="19">
         <v>10</v>
@@ -4126,10 +4126,10 @@
         <v>264</v>
       </c>
       <c r="I5" s="19" t="s">
+        <v>575</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>576</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>577</v>
       </c>
       <c r="K5" s="19">
         <v>10</v>
@@ -4177,10 +4177,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="19" t="s">
+        <v>585</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>586</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>587</v>
       </c>
       <c r="K6" s="19">
         <v>5</v>
@@ -4330,10 +4330,10 @@
         <v>3</v>
       </c>
       <c r="I9" s="21" t="s">
+        <v>579</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>580</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>581</v>
       </c>
       <c r="K9" s="19">
         <v>10</v>
@@ -4459,7 +4459,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="306" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>329</v>
       </c>
@@ -4497,18 +4497,18 @@
         <v>332</v>
       </c>
       <c r="O12" s="23" t="s">
+        <v>600</v>
+      </c>
+      <c r="P12" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="Q12" s="14" t="s">
         <v>334</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>65</v>
@@ -4530,36 +4530,36 @@
         <v>4</v>
       </c>
       <c r="I13" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="K13" s="19">
+        <v>10</v>
+      </c>
+      <c r="L13" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="K13" s="19">
-        <v>10</v>
-      </c>
-      <c r="L13" s="14" t="s">
+      <c r="M13" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="N13" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="N13" s="23" t="s">
+      <c r="O13" s="19" t="s">
         <v>341</v>
       </c>
-      <c r="O13" s="19" t="s">
+      <c r="P13" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="Q13" s="14" t="s">
         <v>343</v>
-      </c>
-      <c r="Q13" s="14" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="191.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>71</v>
@@ -4571,7 +4571,7 @@
         <v>247</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="19" t="s">
@@ -4581,48 +4581,48 @@
         <v>4</v>
       </c>
       <c r="I14" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="J14" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="K14" s="19">
+        <v>10</v>
+      </c>
+      <c r="L14" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="K14" s="19">
-        <v>10</v>
-      </c>
-      <c r="L14" s="14" t="s">
+      <c r="M14" s="14" t="s">
         <v>352</v>
-      </c>
-      <c r="M14" s="14" t="s">
-        <v>353</v>
       </c>
       <c r="N14" s="14" t="s">
         <v>309</v>
       </c>
       <c r="O14" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="P14" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="P14" s="14" t="s">
+      <c r="Q14" s="14" t="s">
         <v>355</v>
-      </c>
-      <c r="Q14" s="14" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>347</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>348</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>247</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="19" t="s">
@@ -4632,36 +4632,36 @@
         <v>4</v>
       </c>
       <c r="I15" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>357</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="K15" s="19">
+        <v>10</v>
+      </c>
+      <c r="L15" s="14" t="s">
         <v>358</v>
       </c>
-      <c r="K15" s="19">
-        <v>10</v>
-      </c>
-      <c r="L15" s="14" t="s">
+      <c r="M15" s="14" t="s">
         <v>359</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>360</v>
       </c>
       <c r="N15" s="14" t="s">
         <v>309</v>
       </c>
       <c r="O15" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="P15" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="P15" s="14" t="s">
+      <c r="Q15" s="14" t="s">
         <v>362</v>
-      </c>
-      <c r="Q15" s="14" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>86</v>
@@ -4673,7 +4673,7 @@
         <v>247</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="19" t="s">
@@ -4683,36 +4683,36 @@
         <v>5</v>
       </c>
       <c r="I16" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="J16" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="J16" s="19" t="s">
-        <v>351</v>
-      </c>
       <c r="K16" s="19">
         <v>10</v>
       </c>
       <c r="L16" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="M16" s="14" t="s">
         <v>372</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>373</v>
       </c>
       <c r="N16" s="14" t="s">
         <v>309</v>
       </c>
       <c r="O16" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="P16" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="Q16" s="14" t="s">
         <v>375</v>
-      </c>
-      <c r="Q16" s="14" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="147.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>90</v>
@@ -4724,7 +4724,7 @@
         <v>247</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="19" t="s">
@@ -4737,33 +4737,33 @@
         <v>93</v>
       </c>
       <c r="J17" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="K17" s="19">
+        <v>10</v>
+      </c>
+      <c r="L17" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="K17" s="19">
-        <v>10</v>
-      </c>
-      <c r="L17" s="14" t="s">
+      <c r="M17" s="14" t="s">
         <v>378</v>
-      </c>
-      <c r="M17" s="14" t="s">
-        <v>379</v>
       </c>
       <c r="N17" s="14" t="s">
         <v>309</v>
       </c>
       <c r="O17" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="P17" s="14" t="s">
         <v>380</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="Q17" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="Q17" s="14" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="216.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>101</v>
@@ -4772,7 +4772,7 @@
         <v>102</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>248</v>
@@ -4785,36 +4785,36 @@
         <v>5</v>
       </c>
       <c r="I18" s="19" t="s">
+        <v>595</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>597</v>
-      </c>
       <c r="K18" s="19">
         <v>10</v>
       </c>
       <c r="L18" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="M18" s="14" t="s">
         <v>383</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>384</v>
       </c>
       <c r="N18" s="14" t="s">
         <v>309</v>
       </c>
       <c r="O18" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="P18" s="14" t="s">
         <v>385</v>
       </c>
-      <c r="P18" s="14" t="s">
+      <c r="Q18" s="14" t="s">
         <v>386</v>
-      </c>
-      <c r="Q18" s="14" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>104</v>
@@ -4823,7 +4823,7 @@
         <v>105</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>248</v>
@@ -4836,36 +4836,36 @@
         <v>5</v>
       </c>
       <c r="I19" s="21" t="s">
+        <v>581</v>
+      </c>
+      <c r="J19" s="19" t="s">
         <v>582</v>
       </c>
-      <c r="J19" s="19" t="s">
-        <v>583</v>
-      </c>
       <c r="K19" s="19">
         <v>10</v>
       </c>
       <c r="L19" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="M19" s="14" t="s">
         <v>388</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>389</v>
       </c>
       <c r="N19" s="14" t="s">
         <v>275</v>
       </c>
       <c r="O19" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="P19" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="P19" s="14" t="s">
+      <c r="Q19" s="14" t="s">
         <v>391</v>
-      </c>
-      <c r="Q19" s="14" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>107</v>
@@ -4874,7 +4874,7 @@
         <v>108</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>248</v>
@@ -4887,36 +4887,36 @@
         <v>5</v>
       </c>
       <c r="I20" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="K20" s="19">
+        <v>10</v>
+      </c>
+      <c r="L20" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="K20" s="19">
-        <v>10</v>
-      </c>
-      <c r="L20" s="14" t="s">
+      <c r="M20" s="14" t="s">
         <v>395</v>
-      </c>
-      <c r="M20" s="14" t="s">
-        <v>396</v>
       </c>
       <c r="N20" s="14" t="s">
         <v>275</v>
       </c>
       <c r="O20" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="P20" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="P20" s="14" t="s">
+      <c r="Q20" s="14" t="s">
         <v>398</v>
-      </c>
-      <c r="Q20" s="14" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>111</v>
@@ -4925,7 +4925,7 @@
         <v>112</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>248</v>
@@ -4947,36 +4947,36 @@
         <v>10</v>
       </c>
       <c r="L21" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="M21" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="N21" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="N21" s="14" t="s">
+      <c r="O21" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="O21" s="14" t="s">
+      <c r="P21" s="14" t="s">
         <v>404</v>
       </c>
-      <c r="P21" s="14" t="s">
+      <c r="Q21" s="14" t="s">
         <v>405</v>
-      </c>
-      <c r="Q21" s="14" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B22" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>368</v>
-      </c>
       <c r="D22" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>248</v>
@@ -4989,45 +4989,45 @@
         <v>5</v>
       </c>
       <c r="I22" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="J22" s="19" t="s">
         <v>584</v>
       </c>
-      <c r="J22" s="19" t="s">
-        <v>585</v>
-      </c>
       <c r="K22" s="19">
         <v>10</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M22" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="N22" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="N22" s="14" t="s">
+      <c r="O22" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="O22" s="14" t="s">
+      <c r="P22" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="P22" s="14" t="s">
+      <c r="Q22" s="14" t="s">
         <v>416</v>
-      </c>
-      <c r="Q22" s="14" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B23" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>369</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>370</v>
-      </c>
       <c r="D23" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>248</v>
@@ -5040,36 +5040,36 @@
         <v>5</v>
       </c>
       <c r="I23" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="J23" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="K23" s="19">
+        <v>10</v>
+      </c>
+      <c r="L23" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="K23" s="19">
-        <v>10</v>
-      </c>
-      <c r="L23" s="14" t="s">
+      <c r="M23" s="19" t="s">
         <v>420</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="N23" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="N23" s="14" t="s">
+      <c r="O23" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="O23" s="14" t="s">
+      <c r="P23" s="14" t="s">
         <v>423</v>
       </c>
-      <c r="P23" s="14" t="s">
+      <c r="Q23" s="14" t="s">
         <v>424</v>
-      </c>
-      <c r="Q23" s="14" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>94</v>
@@ -5081,7 +5081,7 @@
         <v>247</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="19" t="s">
@@ -5091,36 +5091,36 @@
         <v>5</v>
       </c>
       <c r="I24" s="19" t="s">
+        <v>597</v>
+      </c>
+      <c r="J24" s="13" t="s">
         <v>598</v>
       </c>
-      <c r="J24" s="13" t="s">
-        <v>599</v>
-      </c>
       <c r="K24" s="19">
         <v>10</v>
       </c>
       <c r="L24" s="24" t="s">
+        <v>427</v>
+      </c>
+      <c r="M24" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="N24" s="23" t="s">
         <v>429</v>
       </c>
-      <c r="N24" s="23" t="s">
+      <c r="O24" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="O24" s="14" t="s">
+      <c r="P24" s="14" t="s">
         <v>431</v>
       </c>
-      <c r="P24" s="14" t="s">
+      <c r="Q24" s="14" t="s">
         <v>432</v>
-      </c>
-      <c r="Q24" s="14" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>28</v>
@@ -5151,27 +5151,27 @@
         <v>10</v>
       </c>
       <c r="L25" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="M25" s="14" t="s">
         <v>437</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="N25" s="14" t="s">
         <v>438</v>
       </c>
-      <c r="N25" s="14" t="s">
+      <c r="O25" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="O25" s="14" t="s">
+      <c r="P25" s="14" t="s">
         <v>440</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="Q25" s="14" t="s">
         <v>441</v>
-      </c>
-      <c r="Q25" s="14" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="305.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>83</v>
@@ -5193,45 +5193,45 @@
         <v>6</v>
       </c>
       <c r="I26" s="21" t="s">
+        <v>587</v>
+      </c>
+      <c r="J26" s="19" t="s">
         <v>588</v>
-      </c>
-      <c r="J26" s="19" t="s">
-        <v>589</v>
       </c>
       <c r="K26" s="19">
         <v>20</v>
       </c>
       <c r="L26" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="M26" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="N26" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="O26" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="O26" s="14" t="s">
+      <c r="P26" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="P26" s="14" t="s">
+      <c r="Q26" s="14" t="s">
         <v>448</v>
-      </c>
-      <c r="Q26" s="14" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B27" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>435</v>
-      </c>
       <c r="D27" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>248</v>
@@ -5244,31 +5244,31 @@
         <v>6</v>
       </c>
       <c r="I27" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="J27" s="19" t="s">
         <v>450</v>
       </c>
-      <c r="J27" s="19" t="s">
-        <v>451</v>
-      </c>
       <c r="K27" s="19">
         <v>10</v>
       </c>
       <c r="L27" s="14" t="s">
+        <v>452</v>
+      </c>
+      <c r="M27" s="14" t="s">
         <v>453</v>
-      </c>
-      <c r="M27" s="14" t="s">
-        <v>454</v>
       </c>
       <c r="N27" s="14" t="s">
         <v>275</v>
       </c>
       <c r="O27" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="P27" s="14" t="s">
         <v>455</v>
       </c>
-      <c r="P27" s="14" t="s">
+      <c r="Q27" s="14" t="s">
         <v>456</v>
-      </c>
-      <c r="Q27" s="14" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="220.8" x14ac:dyDescent="0.3">
@@ -5285,7 +5285,7 @@
         <v>247</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5" t="s">
@@ -5336,7 +5336,7 @@
         <v>247</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5" t="s">
@@ -5346,10 +5346,10 @@
         <v>264</v>
       </c>
       <c r="I29" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>578</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>579</v>
       </c>
       <c r="K29" s="5">
         <v>10</v>
@@ -5375,7 +5375,7 @@
     </row>
     <row r="30" spans="1:17" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>122</v>
@@ -5387,7 +5387,7 @@
         <v>247</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>249</v>
@@ -5396,36 +5396,36 @@
         <v>1</v>
       </c>
       <c r="I30" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="J30" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>460</v>
-      </c>
       <c r="K30" s="5">
         <v>10</v>
       </c>
       <c r="L30" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="M30" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="N30" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="N30" s="6" t="s">
+      <c r="O30" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="O30" s="6" t="s">
+      <c r="P30" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="P30" s="6" t="s">
+      <c r="Q30" s="6" t="s">
         <v>466</v>
-      </c>
-      <c r="Q30" s="6" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>125</v>
@@ -5437,7 +5437,7 @@
         <v>247</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>249</v>
@@ -5446,31 +5446,31 @@
         <v>1</v>
       </c>
       <c r="I31" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>480</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>481</v>
       </c>
       <c r="K31" s="5">
         <v>5</v>
       </c>
       <c r="L31" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>469</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>470</v>
       </c>
       <c r="N31" s="6" t="s">
         <v>275</v>
       </c>
       <c r="O31" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="P31" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="P31" s="6" t="s">
+      <c r="Q31" s="6" t="s">
         <v>472</v>
-      </c>
-      <c r="Q31" s="6" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="124.2" x14ac:dyDescent="0.3">
@@ -5487,7 +5487,7 @@
         <v>247</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5" t="s">
@@ -5497,10 +5497,10 @@
         <v>2</v>
       </c>
       <c r="I32" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>586</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>587</v>
       </c>
       <c r="K32" s="5">
         <v>5</v>
@@ -5526,7 +5526,7 @@
     </row>
     <row r="33" spans="1:18" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>138</v>
@@ -5538,7 +5538,7 @@
         <v>247</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>249</v>
@@ -5547,16 +5547,16 @@
         <v>2</v>
       </c>
       <c r="I33" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="J33" s="5" t="s">
-        <v>481</v>
-      </c>
       <c r="K33" s="5">
         <v>10</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M33" s="6" t="s">
         <v>308</v>
@@ -5565,18 +5565,18 @@
         <v>275</v>
       </c>
       <c r="O33" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="P33" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="P33" s="9" t="s">
+      <c r="Q33" s="6" t="s">
         <v>477</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>141</v>
@@ -5588,7 +5588,7 @@
         <v>247</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>249</v>
@@ -5597,36 +5597,36 @@
         <v>2</v>
       </c>
       <c r="I34" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5">
+        <v>10</v>
+      </c>
+      <c r="L34" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="K34" s="5">
-        <v>10</v>
-      </c>
-      <c r="L34" s="6" t="s">
+      <c r="M34" s="6" t="s">
         <v>482</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>483</v>
       </c>
       <c r="N34" s="6" t="s">
         <v>275</v>
       </c>
       <c r="O34" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="P34" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="P34" s="6" t="s">
+      <c r="Q34" s="6" t="s">
         <v>485</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="273.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>129</v>
@@ -5638,7 +5638,7 @@
         <v>247</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>249</v>
@@ -5647,39 +5647,39 @@
         <v>3</v>
       </c>
       <c r="I35" s="18" t="s">
+        <v>577</v>
+      </c>
+      <c r="J35" s="13" t="s">
         <v>578</v>
       </c>
-      <c r="J35" s="13" t="s">
-        <v>579</v>
-      </c>
       <c r="K35" s="5">
         <v>10</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>308</v>
       </c>
       <c r="N35" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="O35" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="O35" s="6" t="s">
+      <c r="P35" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="P35" s="6" t="s">
+      <c r="Q35" s="6" t="s">
         <v>491</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>152</v>
@@ -5688,7 +5688,7 @@
         <v>247</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>249</v>
@@ -5697,36 +5697,36 @@
         <v>3</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J36" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="K36" s="5">
+        <v>10</v>
+      </c>
+      <c r="L36" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="K36" s="5">
-        <v>10</v>
-      </c>
-      <c r="L36" s="6" t="s">
+      <c r="M36" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="M36" s="6" t="s">
+      <c r="N36" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="N36" s="6" t="s">
+      <c r="O36" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="O36" s="6" t="s">
+      <c r="P36" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="P36" s="6" t="s">
+      <c r="Q36" s="6" t="s">
         <v>501</v>
-      </c>
-      <c r="Q36" s="6" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="271.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>144</v>
@@ -5738,7 +5738,7 @@
         <v>247</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>249</v>
@@ -5750,45 +5750,45 @@
         <v>147</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K37" s="5">
         <v>10</v>
       </c>
       <c r="L37" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="M37" s="6" t="s">
         <v>504</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>505</v>
       </c>
       <c r="N37" s="6" t="s">
         <v>275</v>
       </c>
       <c r="O37" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="P37" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="P37" s="6" t="s">
+      <c r="Q37" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="Q37" s="6" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="211.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>247</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>249</v>
@@ -5797,39 +5797,39 @@
         <v>4</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K38" s="5">
         <v>10</v>
       </c>
       <c r="L38" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="M38" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="M38" s="6" t="s">
+      <c r="N38" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="N38" s="6" t="s">
+      <c r="O38" s="8" t="s">
         <v>517</v>
       </c>
-      <c r="O38" s="8" t="s">
+      <c r="P38" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="P38" s="6" t="s">
+      <c r="Q38" s="6" t="s">
         <v>519</v>
-      </c>
-      <c r="Q38" s="6" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="260.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>156</v>
@@ -5838,7 +5838,7 @@
         <v>247</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>249</v>
@@ -5847,48 +5847,48 @@
         <v>4</v>
       </c>
       <c r="I39" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>459</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>460</v>
       </c>
       <c r="K39" s="5">
         <v>15</v>
       </c>
       <c r="L39" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="M39" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="M39" s="6" t="s">
+      <c r="N39" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="O39" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="N39" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="O39" s="6" t="s">
+      <c r="P39" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="P39" s="6" t="s">
+      <c r="Q39" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="Q39" s="6" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>247</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>249</v>
@@ -5902,27 +5902,27 @@
         <v>5</v>
       </c>
       <c r="L40" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="M40" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="M40" s="6" t="s">
+      <c r="N40" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="N40" s="6" t="s">
+      <c r="O40" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="O40" s="6" t="s">
+      <c r="P40" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="P40" s="6" t="s">
+      <c r="Q40" s="6" t="s">
         <v>532</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>165</v>
@@ -5934,7 +5934,7 @@
         <v>247</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>249</v>
@@ -5943,36 +5943,36 @@
         <v>5</v>
       </c>
       <c r="I41" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="J41" s="5" t="s">
         <v>535</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>536</v>
       </c>
       <c r="K41" s="5">
         <v>20</v>
       </c>
       <c r="L41" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="M41" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="M41" s="6" t="s">
-        <v>538</v>
-      </c>
       <c r="N41" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="O41" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="O41" s="6" t="s">
+      <c r="P41" s="6" t="s">
         <v>541</v>
       </c>
-      <c r="P41" s="6" t="s">
+      <c r="Q41" s="6" t="s">
         <v>542</v>
-      </c>
-      <c r="Q41" s="6" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="153" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>104</v>
@@ -5981,10 +5981,10 @@
         <v>105</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>249</v>
@@ -5993,48 +5993,48 @@
         <v>5</v>
       </c>
       <c r="I42" s="18" t="s">
+        <v>581</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="J42" s="5" t="s">
-        <v>583</v>
-      </c>
       <c r="K42" s="5">
         <v>10</v>
       </c>
       <c r="L42" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="M42" s="6" t="s">
         <v>388</v>
-      </c>
-      <c r="M42" s="6" t="s">
-        <v>389</v>
       </c>
       <c r="N42" s="6" t="s">
         <v>275</v>
       </c>
       <c r="O42" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="P42" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="P42" s="6" t="s">
+      <c r="Q42" s="6" t="s">
         <v>391</v>
-      </c>
-      <c r="Q42" s="6" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>368</v>
-      </c>
       <c r="D43" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>249</v>
@@ -6043,49 +6043,49 @@
         <v>5</v>
       </c>
       <c r="I43" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="J43" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="J43" s="5" t="s">
-        <v>585</v>
-      </c>
       <c r="K43" s="5">
         <v>10</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M43" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="N43" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="N43" s="6" t="s">
+      <c r="O43" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="O43" s="6" t="s">
+      <c r="P43" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="P43" s="6" t="s">
+      <c r="Q43" s="6" t="s">
         <v>416</v>
-      </c>
-      <c r="Q43" s="6" t="s">
-        <v>417</v>
       </c>
       <c r="R43" s="6"/>
     </row>
     <row r="44" spans="1:18" ht="138" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>370</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>249</v>
@@ -6094,36 +6094,36 @@
         <v>5</v>
       </c>
       <c r="I44" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J44" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="K44" s="5">
+        <v>10</v>
+      </c>
+      <c r="L44" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="K44" s="5">
-        <v>10</v>
-      </c>
-      <c r="L44" s="6" t="s">
+      <c r="M44" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="N44" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="N44" s="6" t="s">
+      <c r="O44" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="O44" s="6" t="s">
+      <c r="P44" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="P44" s="6" t="s">
+      <c r="Q44" s="6" t="s">
         <v>424</v>
-      </c>
-      <c r="Q44" s="6" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="345" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>174</v>
@@ -6132,10 +6132,10 @@
         <v>175</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>249</v>
@@ -6147,45 +6147,45 @@
         <v>177</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="K45" s="5">
         <v>10</v>
       </c>
       <c r="L45" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>546</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>547</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>275</v>
       </c>
       <c r="O45" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="P45" s="6" t="s">
         <v>548</v>
       </c>
-      <c r="P45" s="6" t="s">
+      <c r="Q45" s="6" t="s">
         <v>549</v>
-      </c>
-      <c r="Q45" s="6" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="358.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>249</v>
@@ -6194,36 +6194,36 @@
         <v>5</v>
       </c>
       <c r="I46" s="18" t="s">
+        <v>591</v>
+      </c>
+      <c r="J46" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="J46" s="5" t="s">
-        <v>593</v>
-      </c>
       <c r="K46" s="5">
         <v>10</v>
       </c>
       <c r="L46" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="M46" s="6" t="s">
         <v>553</v>
       </c>
-      <c r="M46" s="6" t="s">
+      <c r="N46" s="6" t="s">
         <v>554</v>
       </c>
-      <c r="N46" s="6" t="s">
+      <c r="O46" s="6" t="s">
         <v>555</v>
       </c>
-      <c r="O46" s="6" t="s">
+      <c r="P46" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="P46" s="6" t="s">
+      <c r="Q46" s="6" t="s">
         <v>557</v>
-      </c>
-      <c r="Q46" s="6" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="214.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>131</v>
@@ -6235,7 +6235,7 @@
         <v>247</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>249</v>
@@ -6249,27 +6249,27 @@
         <v>10</v>
       </c>
       <c r="L47" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="M47" s="6" t="s">
+      <c r="N47" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="N47" s="6" t="s">
+      <c r="O47" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="O47" s="6" t="s">
+      <c r="P47" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="P47" s="6" t="s">
+      <c r="Q47" s="6" t="s">
         <v>563</v>
-      </c>
-      <c r="Q47" s="6" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="267.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>163</v>
@@ -6281,7 +6281,7 @@
         <v>247</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>249</v>
@@ -6290,48 +6290,48 @@
         <v>6</v>
       </c>
       <c r="I48" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>594</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>595</v>
       </c>
       <c r="K48" s="5">
         <v>20</v>
       </c>
       <c r="L48" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="M48" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="M48" s="6" t="s">
+      <c r="N48" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="N48" s="6" t="s">
+      <c r="O48" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="O48" s="6" t="s">
+      <c r="P48" s="6" t="s">
         <v>570</v>
       </c>
-      <c r="P48" s="6" t="s">
+      <c r="Q48" s="6" t="s">
         <v>571</v>
-      </c>
-      <c r="Q48" s="6" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>435</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>249</v>
@@ -6340,31 +6340,31 @@
         <v>6</v>
       </c>
       <c r="I49" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="J49" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="J49" s="5" t="s">
-        <v>451</v>
-      </c>
       <c r="K49" s="5">
         <v>10</v>
       </c>
       <c r="L49" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>453</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>454</v>
       </c>
       <c r="N49" s="6" t="s">
         <v>275</v>
       </c>
       <c r="O49" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="P49" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="P49" s="6" t="s">
+      <c r="Q49" s="6" t="s">
         <v>456</v>
-      </c>
-      <c r="Q49" s="6" t="s">
-        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -6760,12 +6760,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6927,15 +6924,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57723507-2D03-46ED-A005-5642ABE4AB7F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6959,16 +6966,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57723507-2D03-46ED-A005-5642ABE4AB7F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
bindestrek med for bedre søk
</commit_message>
<xml_diff>
--- a/Diku.xlsx
+++ b/Diku.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\OneDrive\Dokumenter\DIKU\DIKU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F71400-E054-4E62-80DB-CF6F8D1B72DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB8D6BE-1744-4DB9-BB77-1FA7EB54C420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1863,7 +1863,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1925,12 +1925,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1969,57 +1963,35 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -2030,6 +2002,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3871,8 +3850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCDD31-3723-4F19-8F81-7049F051B343}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K11" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="M28" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3889,7 +3868,7 @@
     <col min="10" max="10" width="22.88671875" customWidth="1"/>
     <col min="11" max="11" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="55.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="51.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="65.77734375" customWidth="1"/>
     <col min="16" max="16" width="48.77734375" customWidth="1"/>
@@ -3897,2473 +3876,2492 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="7" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="325.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="11">
         <v>1</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="K2" s="19">
-        <v>10</v>
-      </c>
-      <c r="L2" s="14" t="s">
+      <c r="K2" s="11">
+        <v>10</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="8" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="301.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="11">
         <v>1</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="11" t="s">
         <v>573</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="11" t="s">
         <v>574</v>
       </c>
-      <c r="K3" s="19">
-        <v>10</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="K3" s="11">
+        <v>10</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="P3" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="12" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="11">
         <v>1</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="11">
         <v>5</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="Q4" s="12" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="326.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="11" t="s">
         <v>575</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="11" t="s">
         <v>576</v>
       </c>
-      <c r="K5" s="19">
-        <v>10</v>
-      </c>
-      <c r="L5" s="14" t="s">
+      <c r="K5" s="11">
+        <v>10</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="Q5" s="12" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="11">
         <v>2</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="11" t="s">
         <v>585</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="11" t="s">
         <v>586</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="11">
         <v>5</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="P6" s="20" t="s">
+      <c r="P6" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="Q6" s="20" t="s">
+      <c r="Q6" s="12" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="202.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="11">
         <v>2</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="K7" s="19">
-        <v>10</v>
-      </c>
-      <c r="L7" s="14" t="s">
+      <c r="K7" s="11">
+        <v>10</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="P7" s="20" t="s">
+      <c r="P7" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="Q7" s="12" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="11">
         <v>2</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="K8" s="19">
-        <v>10</v>
-      </c>
-      <c r="L8" s="14" t="s">
+      <c r="K8" s="11">
+        <v>10</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="O8" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="Q8" s="11" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="388.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="11">
         <v>3</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="13" t="s">
         <v>579</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="11" t="s">
         <v>580</v>
       </c>
-      <c r="K9" s="19">
-        <v>10</v>
-      </c>
-      <c r="L9" s="14" t="s">
+      <c r="K9" s="11">
+        <v>10</v>
+      </c>
+      <c r="L9" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="N9" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O9" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="P9" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" s="8" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="19" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="11">
         <v>3</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="K10" s="19">
-        <v>10</v>
-      </c>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="11">
+        <v>10</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="O10" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="P10" s="23" t="s">
+      <c r="P10" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="Q10" s="23" t="s">
+      <c r="Q10" s="15" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="19" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="11">
         <v>3</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="K11" s="19">
-        <v>10</v>
-      </c>
-      <c r="L11" s="14" t="s">
+      <c r="K11" s="11">
+        <v>10</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M11" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O11" s="19" t="s">
+      <c r="O11" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="8" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="306" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="19" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="11">
         <v>4</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="19">
-        <v>10</v>
-      </c>
-      <c r="L12" s="14" t="s">
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="11">
+        <v>10</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="O12" s="23" t="s">
+      <c r="O12" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="8" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="11">
         <v>4</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="K13" s="19">
-        <v>10</v>
-      </c>
-      <c r="L13" s="14" t="s">
+      <c r="K13" s="11">
+        <v>10</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="M13" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="N13" s="23" t="s">
+      <c r="N13" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="O13" s="19" t="s">
+      <c r="O13" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="Q13" s="14" t="s">
+      <c r="Q13" s="8" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="191.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="19" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="11">
         <v>4</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="K14" s="19">
-        <v>10</v>
-      </c>
-      <c r="L14" s="14" t="s">
+      <c r="K14" s="11">
+        <v>10</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="N14" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="O14" s="19" t="s">
+      <c r="O14" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="P14" s="14" t="s">
+      <c r="P14" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="Q14" s="14" t="s">
+      <c r="Q14" s="8" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="19" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="11">
         <v>4</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="K15" s="19">
-        <v>10</v>
-      </c>
-      <c r="L15" s="14" t="s">
+      <c r="K15" s="11">
+        <v>10</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="N15" s="14" t="s">
+      <c r="N15" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="O15" s="14" t="s">
+      <c r="O15" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="P15" s="14" t="s">
+      <c r="P15" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="8" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="19" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="11">
         <v>5</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="K16" s="19">
-        <v>10</v>
-      </c>
-      <c r="L16" s="14" t="s">
+      <c r="K16" s="11">
+        <v>10</v>
+      </c>
+      <c r="L16" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="N16" s="14" t="s">
+      <c r="N16" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="O16" s="14" t="s">
+      <c r="O16" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="P16" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="Q16" s="8" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="147.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="19" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="11">
         <v>5</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="K17" s="19">
-        <v>10</v>
-      </c>
-      <c r="L17" s="14" t="s">
+      <c r="K17" s="11">
+        <v>10</v>
+      </c>
+      <c r="L17" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="O17" s="14" t="s">
+      <c r="O17" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="P17" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="8" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="216.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="19" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="11">
         <v>5</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="11" t="s">
         <v>595</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="11" t="s">
         <v>596</v>
       </c>
-      <c r="K18" s="19">
-        <v>10</v>
-      </c>
-      <c r="L18" s="14" t="s">
+      <c r="K18" s="11">
+        <v>10</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="N18" s="14" t="s">
+      <c r="N18" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="O18" s="14" t="s">
+      <c r="O18" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="P18" s="14" t="s">
+      <c r="P18" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="Q18" s="14" t="s">
+      <c r="Q18" s="8" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="19" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="11">
         <v>5</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="11" t="s">
         <v>582</v>
       </c>
-      <c r="K19" s="19">
-        <v>10</v>
-      </c>
-      <c r="L19" s="14" t="s">
+      <c r="K19" s="11">
+        <v>10</v>
+      </c>
+      <c r="L19" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="N19" s="14" t="s">
+      <c r="N19" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O19" s="14" t="s">
+      <c r="O19" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="P19" s="14" t="s">
+      <c r="P19" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="Q19" s="14" t="s">
+      <c r="Q19" s="8" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="19" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="11">
         <v>5</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="K20" s="19">
-        <v>10</v>
-      </c>
-      <c r="L20" s="14" t="s">
+      <c r="K20" s="11">
+        <v>10</v>
+      </c>
+      <c r="L20" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O20" s="14" t="s">
+      <c r="O20" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="P20" s="14" t="s">
+      <c r="P20" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="Q20" s="14" t="s">
+      <c r="Q20" s="8" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="19" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="11">
         <v>5</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="K21" s="19">
-        <v>10</v>
-      </c>
-      <c r="L21" s="14" t="s">
+      <c r="K21" s="11">
+        <v>10</v>
+      </c>
+      <c r="L21" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="N21" s="14" t="s">
+      <c r="N21" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="O21" s="14" t="s">
+      <c r="O21" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="P21" s="14" t="s">
+      <c r="P21" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="Q21" s="14" t="s">
+      <c r="Q21" s="8" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="403.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="19" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="11">
         <v>5</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="11" t="s">
         <v>583</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="11" t="s">
         <v>584</v>
       </c>
-      <c r="K22" s="19">
-        <v>10</v>
-      </c>
-      <c r="L22" s="14" t="s">
+      <c r="K22" s="11">
+        <v>10</v>
+      </c>
+      <c r="L22" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="N22" s="14" t="s">
+      <c r="N22" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="O22" s="14" t="s">
+      <c r="O22" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="P22" s="14" t="s">
+      <c r="P22" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="Q22" s="14" t="s">
+      <c r="Q22" s="8" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="19" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="11">
         <v>5</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="K23" s="19">
-        <v>10</v>
-      </c>
-      <c r="L23" s="14" t="s">
+      <c r="K23" s="11">
+        <v>10</v>
+      </c>
+      <c r="L23" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="M23" s="11" t="s">
         <v>420</v>
       </c>
-      <c r="N23" s="14" t="s">
+      <c r="N23" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="O23" s="14" t="s">
+      <c r="O23" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="P23" s="14" t="s">
+      <c r="P23" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="Q23" s="14" t="s">
+      <c r="Q23" s="8" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="19" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="11">
         <v>5</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="11" t="s">
         <v>597</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="14" t="s">
         <v>598</v>
       </c>
-      <c r="K24" s="19">
-        <v>10</v>
-      </c>
-      <c r="L24" s="24" t="s">
+      <c r="K24" s="11">
+        <v>10</v>
+      </c>
+      <c r="L24" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="M24" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="N24" s="23" t="s">
+      <c r="N24" s="15" t="s">
         <v>429</v>
       </c>
-      <c r="O24" s="14" t="s">
+      <c r="O24" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="P24" s="14" t="s">
+      <c r="P24" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="Q24" s="14" t="s">
+      <c r="Q24" s="8" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="19" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H25" s="11">
         <v>6</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="K25" s="19">
-        <v>10</v>
-      </c>
-      <c r="L25" s="14" t="s">
+      <c r="K25" s="11">
+        <v>10</v>
+      </c>
+      <c r="L25" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="N25" s="14" t="s">
+      <c r="N25" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="O25" s="14" t="s">
+      <c r="O25" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="P25" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="Q25" s="14" t="s">
+      <c r="Q25" s="8" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="305.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="19" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="11">
         <v>6</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="13" t="s">
         <v>587</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="11" t="s">
         <v>588</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="11">
         <v>20</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="L26" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="M26" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="N26" s="14" t="s">
+      <c r="N26" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="O26" s="14" t="s">
+      <c r="O26" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="P26" s="14" t="s">
+      <c r="P26" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="Q26" s="14" t="s">
+      <c r="Q26" s="8" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="19" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="11">
         <v>6</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="J27" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="K27" s="19">
-        <v>10</v>
-      </c>
-      <c r="L27" s="14" t="s">
+      <c r="K27" s="11">
+        <v>10</v>
+      </c>
+      <c r="L27" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="N27" s="14" t="s">
+      <c r="N27" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O27" s="14" t="s">
+      <c r="O27" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="P27" s="14" t="s">
+      <c r="P27" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q27" s="14" t="s">
+      <c r="Q27" s="8" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="220.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:17" ht="216" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5" t="s">
+      <c r="F28" s="11"/>
+      <c r="G28" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="11">
         <v>1</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="K28" s="5">
-        <v>10</v>
-      </c>
-      <c r="L28" s="6" t="s">
+      <c r="K28" s="11">
+        <v>10</v>
+      </c>
+      <c r="L28" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="M28" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="N28" s="6" t="s">
+      <c r="N28" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="O28" s="5" t="s">
+      <c r="O28" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="P28" s="6" t="s">
+      <c r="P28" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="Q28" s="6" t="s">
+      <c r="Q28" s="8" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="276" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="11" t="s">
         <v>577</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J29" s="11" t="s">
         <v>578</v>
       </c>
-      <c r="K29" s="5">
-        <v>10</v>
-      </c>
-      <c r="L29" s="6" t="s">
+      <c r="K29" s="11">
+        <v>10</v>
+      </c>
+      <c r="L29" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="M29" s="6" t="s">
+      <c r="M29" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="N29" s="6" t="s">
+      <c r="N29" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="O29" s="5" t="s">
+      <c r="O29" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="P29" s="10" t="s">
+      <c r="P29" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="Q29" s="10" t="s">
+      <c r="Q29" s="12" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="F30" s="10"/>
+      <c r="G30" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="18">
         <v>1</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="I30" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="K30" s="5">
-        <v>10</v>
-      </c>
-      <c r="L30" s="6" t="s">
+      <c r="K30" s="11">
+        <v>10</v>
+      </c>
+      <c r="L30" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="M30" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="N30" s="6" t="s">
+      <c r="N30" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="O30" s="6" t="s">
+      <c r="O30" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="P30" s="6" t="s">
+      <c r="P30" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="Q30" s="8" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>467</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="18">
         <v>1</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J31" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="K31" s="5">
+      <c r="K31" s="11">
         <v>5</v>
       </c>
-      <c r="L31" s="6" t="s">
+      <c r="L31" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="M31" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="N31" s="6" t="s">
+      <c r="N31" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O31" s="6" t="s">
+      <c r="O31" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="P31" s="6" t="s">
+      <c r="P31" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="Q31" s="6" t="s">
+      <c r="Q31" s="8" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5" t="s">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="11">
         <v>2</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="11" t="s">
         <v>585</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" s="11" t="s">
         <v>586</v>
       </c>
-      <c r="K32" s="5">
+      <c r="K32" s="11">
         <v>5</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="L32" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="M32" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="N32" s="6" t="s">
+      <c r="N32" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="O32" s="5" t="s">
+      <c r="O32" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="P32" s="10" t="s">
+      <c r="P32" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="Q32" s="10" t="s">
+      <c r="Q32" s="12" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="F33" s="10"/>
+      <c r="G33" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="11">
         <v>2</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="K33" s="5">
-        <v>10</v>
-      </c>
-      <c r="L33" s="6" t="s">
+      <c r="K33" s="11">
+        <v>10</v>
+      </c>
+      <c r="L33" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="M33" s="6" t="s">
+      <c r="M33" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="N33" s="6" t="s">
+      <c r="N33" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O33" s="6" t="s">
+      <c r="O33" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="P33" s="9" t="s">
+      <c r="P33" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="Q33" s="6" t="s">
+      <c r="Q33" s="8" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="220.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:18" ht="216" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>478</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="F34" s="10"/>
+      <c r="G34" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H34" s="5">
+      <c r="H34" s="11">
         <v>2</v>
       </c>
-      <c r="I34" s="16" t="s">
+      <c r="I34" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="K34" s="5">
-        <v>10</v>
-      </c>
-      <c r="L34" s="6" t="s">
+      <c r="K34" s="11">
+        <v>10</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="M34" s="6" t="s">
+      <c r="M34" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="N34" s="6" t="s">
+      <c r="N34" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O34" s="6" t="s">
+      <c r="O34" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="P34" s="6" t="s">
+      <c r="P34" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="Q34" s="6" t="s">
+      <c r="Q34" s="8" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="273.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="F35" s="10"/>
+      <c r="G35" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="11">
         <v>3</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I35" s="13" t="s">
         <v>577</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="14" t="s">
         <v>578</v>
       </c>
-      <c r="K35" s="5">
-        <v>10</v>
-      </c>
-      <c r="L35" s="6" t="s">
+      <c r="K35" s="11">
+        <v>10</v>
+      </c>
+      <c r="L35" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="M35" s="6" t="s">
+      <c r="M35" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="N35" s="6" t="s">
+      <c r="N35" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="O35" s="6" t="s">
+      <c r="O35" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="P35" s="6" t="s">
+      <c r="P35" s="8" t="s">
         <v>490</v>
       </c>
-      <c r="Q35" s="6" t="s">
+      <c r="Q35" s="8" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="198" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="11" t="s">
         <v>494</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="11" t="s">
         <v>492</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H36" s="11">
         <v>3</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="J36" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="K36" s="5">
-        <v>10</v>
-      </c>
-      <c r="L36" s="6" t="s">
+      <c r="K36" s="11">
+        <v>10</v>
+      </c>
+      <c r="L36" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="M36" s="6" t="s">
+      <c r="M36" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="N36" s="6" t="s">
+      <c r="N36" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="O36" s="6" t="s">
+      <c r="O36" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="P36" s="6" t="s">
+      <c r="P36" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="Q36" s="6" t="s">
+      <c r="Q36" s="8" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="271.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="11" t="s">
         <v>502</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="F37" s="10"/>
+      <c r="G37" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H37" s="11">
         <v>3</v>
       </c>
-      <c r="I37" s="18" t="s">
+      <c r="I37" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J37" s="11" t="s">
         <v>589</v>
       </c>
-      <c r="K37" s="5">
-        <v>10</v>
-      </c>
-      <c r="L37" s="6" t="s">
+      <c r="K37" s="11">
+        <v>10</v>
+      </c>
+      <c r="L37" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="M37" s="6" t="s">
+      <c r="M37" s="8" t="s">
         <v>504</v>
       </c>
-      <c r="N37" s="6" t="s">
+      <c r="N37" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O37" s="6" t="s">
+      <c r="O37" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="P37" s="6" t="s">
+      <c r="P37" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="Q37" s="6" t="s">
+      <c r="Q37" s="8" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="211.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="11" t="s">
         <v>513</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="F38" s="10"/>
+      <c r="G38" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="11">
         <v>4</v>
       </c>
-      <c r="I38" s="6" t="s">
+      <c r="I38" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="K38" s="5">
-        <v>10</v>
-      </c>
-      <c r="L38" s="6" t="s">
+      <c r="K38" s="11">
+        <v>10</v>
+      </c>
+      <c r="L38" s="8" t="s">
         <v>514</v>
       </c>
-      <c r="M38" s="6" t="s">
+      <c r="M38" s="8" t="s">
         <v>515</v>
       </c>
-      <c r="N38" s="6" t="s">
+      <c r="N38" s="8" t="s">
         <v>516</v>
       </c>
-      <c r="O38" s="8" t="s">
+      <c r="O38" s="15" t="s">
         <v>517</v>
       </c>
-      <c r="P38" s="6" t="s">
+      <c r="P38" s="8" t="s">
         <v>518</v>
       </c>
-      <c r="Q38" s="6" t="s">
+      <c r="Q38" s="8" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="260.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="F39" s="10"/>
+      <c r="G39" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="11">
         <v>4</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="I39" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="K39" s="5">
+      <c r="K39" s="11">
         <v>15</v>
       </c>
-      <c r="L39" s="6" t="s">
+      <c r="L39" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="M39" s="6" t="s">
+      <c r="M39" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="N39" s="6" t="s">
+      <c r="N39" s="8" t="s">
         <v>538</v>
       </c>
-      <c r="O39" s="6" t="s">
+      <c r="O39" s="8" t="s">
         <v>523</v>
       </c>
-      <c r="P39" s="6" t="s">
+      <c r="P39" s="8" t="s">
         <v>524</v>
       </c>
-      <c r="Q39" s="6" t="s">
+      <c r="Q39" s="8" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="11" t="s">
         <v>526</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="F40" s="10"/>
+      <c r="G40" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H40" s="11">
         <v>4</v>
       </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="5">
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="11">
         <v>5</v>
       </c>
-      <c r="L40" s="6" t="s">
+      <c r="L40" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="M40" s="6" t="s">
+      <c r="M40" s="8" t="s">
         <v>528</v>
       </c>
-      <c r="N40" s="6" t="s">
+      <c r="N40" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="O40" s="6" t="s">
+      <c r="O40" s="8" t="s">
         <v>530</v>
       </c>
-      <c r="P40" s="6" t="s">
+      <c r="P40" s="8" t="s">
         <v>531</v>
       </c>
-      <c r="Q40" s="6" t="s">
+      <c r="Q40" s="8" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="234.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:18" ht="216" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
         <v>533</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="F41" s="10"/>
+      <c r="G41" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H41" s="11">
         <v>5</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="I41" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="J41" s="5" t="s">
+      <c r="J41" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="K41" s="5">
+      <c r="K41" s="11">
         <v>20</v>
       </c>
-      <c r="L41" s="6" t="s">
+      <c r="L41" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="M41" s="6" t="s">
+      <c r="M41" s="8" t="s">
         <v>537</v>
       </c>
-      <c r="N41" s="6" t="s">
+      <c r="N41" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="O41" s="6" t="s">
+      <c r="O41" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="P41" s="6" t="s">
+      <c r="P41" s="8" t="s">
         <v>541</v>
       </c>
-      <c r="Q41" s="6" t="s">
+      <c r="Q41" s="8" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="153" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="F42" s="10"/>
+      <c r="G42" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="11">
         <v>5</v>
       </c>
-      <c r="I42" s="18" t="s">
+      <c r="I42" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J42" s="11" t="s">
         <v>582</v>
       </c>
-      <c r="K42" s="5">
-        <v>10</v>
-      </c>
-      <c r="L42" s="6" t="s">
+      <c r="K42" s="11">
+        <v>10</v>
+      </c>
+      <c r="L42" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="M42" s="6" t="s">
+      <c r="M42" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="N42" s="6" t="s">
+      <c r="N42" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O42" s="6" t="s">
+      <c r="O42" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="P42" s="6" t="s">
+      <c r="P42" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="Q42" s="6" t="s">
+      <c r="Q42" s="8" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:18" ht="403.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="F43" s="10"/>
+      <c r="G43" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H43" s="11">
         <v>5</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I43" s="11" t="s">
         <v>583</v>
       </c>
-      <c r="J43" s="5" t="s">
+      <c r="J43" s="11" t="s">
         <v>584</v>
       </c>
-      <c r="K43" s="5">
-        <v>10</v>
-      </c>
-      <c r="L43" s="6" t="s">
+      <c r="K43" s="11">
+        <v>10</v>
+      </c>
+      <c r="L43" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="M43" s="6" t="s">
+      <c r="M43" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="N43" s="6" t="s">
+      <c r="N43" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="O43" s="6" t="s">
+      <c r="O43" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="P43" s="6" t="s">
+      <c r="P43" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="Q43" s="6" t="s">
+      <c r="Q43" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="R43" s="6"/>
-    </row>
-    <row r="44" spans="1:18" ht="138" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="R43" s="5"/>
+    </row>
+    <row r="44" spans="1:18" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="F44" s="10"/>
+      <c r="G44" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H44" s="5">
+      <c r="H44" s="11">
         <v>5</v>
       </c>
-      <c r="I44" s="12" t="s">
+      <c r="I44" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="K44" s="5">
-        <v>10</v>
-      </c>
-      <c r="L44" s="6" t="s">
+      <c r="K44" s="11">
+        <v>10</v>
+      </c>
+      <c r="L44" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="M44" s="11" t="s">
         <v>420</v>
       </c>
-      <c r="N44" s="6" t="s">
+      <c r="N44" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="O44" s="6" t="s">
+      <c r="O44" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="P44" s="6" t="s">
+      <c r="P44" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="Q44" s="6" t="s">
+      <c r="Q44" s="8" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="345" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:18" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
         <v>544</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="F45" s="10"/>
+      <c r="G45" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H45" s="5">
+      <c r="H45" s="11">
         <v>5</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="I45" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J45" s="11" t="s">
         <v>590</v>
       </c>
-      <c r="K45" s="5">
-        <v>10</v>
-      </c>
-      <c r="L45" s="6" t="s">
+      <c r="K45" s="11">
+        <v>10</v>
+      </c>
+      <c r="L45" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="M45" s="6" t="s">
+      <c r="M45" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="N45" s="6" t="s">
+      <c r="N45" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O45" s="6" t="s">
+      <c r="O45" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="P45" s="6" t="s">
+      <c r="P45" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="Q45" s="6" t="s">
+      <c r="Q45" s="8" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="358.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:18" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="11" t="s">
         <v>550</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="F46" s="10"/>
+      <c r="G46" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H46" s="5">
+      <c r="H46" s="11">
         <v>5</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="I46" s="13" t="s">
         <v>591</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="J46" s="11" t="s">
         <v>592</v>
       </c>
-      <c r="K46" s="5">
-        <v>10</v>
-      </c>
-      <c r="L46" s="6" t="s">
+      <c r="K46" s="11">
+        <v>10</v>
+      </c>
+      <c r="L46" s="8" t="s">
         <v>552</v>
       </c>
-      <c r="M46" s="6" t="s">
+      <c r="M46" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="N46" s="6" t="s">
+      <c r="N46" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="O46" s="6" t="s">
+      <c r="O46" s="8" t="s">
         <v>555</v>
       </c>
-      <c r="P46" s="6" t="s">
+      <c r="P46" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="Q46" s="6" t="s">
+      <c r="Q46" s="8" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="214.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="11" t="s">
         <v>564</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="F47" s="10"/>
+      <c r="G47" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H47" s="5">
+      <c r="H47" s="11">
         <v>6</v>
       </c>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="5">
-        <v>10</v>
-      </c>
-      <c r="L47" s="6" t="s">
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="11">
+        <v>10</v>
+      </c>
+      <c r="L47" s="8" t="s">
         <v>558</v>
       </c>
-      <c r="M47" s="6" t="s">
+      <c r="M47" s="8" t="s">
         <v>559</v>
       </c>
-      <c r="N47" s="6" t="s">
+      <c r="N47" s="8" t="s">
         <v>560</v>
       </c>
-      <c r="O47" s="6" t="s">
+      <c r="O47" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="P47" s="6" t="s">
+      <c r="P47" s="8" t="s">
         <v>562</v>
       </c>
-      <c r="Q47" s="6" t="s">
+      <c r="Q47" s="8" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="267.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="11" t="s">
         <v>565</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="F48" s="10"/>
+      <c r="G48" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H48" s="5">
+      <c r="H48" s="11">
         <v>6</v>
       </c>
-      <c r="I48" s="18" t="s">
+      <c r="I48" s="13" t="s">
         <v>593</v>
       </c>
-      <c r="J48" s="5" t="s">
+      <c r="J48" s="11" t="s">
         <v>594</v>
       </c>
-      <c r="K48" s="5">
+      <c r="K48" s="11">
         <v>20</v>
       </c>
-      <c r="L48" s="6" t="s">
+      <c r="L48" s="8" t="s">
         <v>566</v>
       </c>
-      <c r="M48" s="6" t="s">
+      <c r="M48" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="N48" s="6" t="s">
+      <c r="N48" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="O48" s="6" t="s">
+      <c r="O48" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="P48" s="6" t="s">
+      <c r="P48" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="Q48" s="6" t="s">
+      <c r="Q48" s="8" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="F49" s="10"/>
+      <c r="G49" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H49" s="5">
+      <c r="H49" s="11">
         <v>6</v>
       </c>
-      <c r="I49" s="12" t="s">
+      <c r="I49" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J49" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="K49" s="5">
-        <v>10</v>
-      </c>
-      <c r="L49" s="6" t="s">
+      <c r="K49" s="11">
+        <v>10</v>
+      </c>
+      <c r="L49" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="M49" s="6" t="s">
+      <c r="M49" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="N49" s="6" t="s">
+      <c r="N49" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="O49" s="6" t="s">
+      <c r="O49" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="P49" s="6" t="s">
+      <c r="P49" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q49" s="6" t="s">
+      <c r="Q49" s="8" t="s">
         <v>456</v>
       </c>
     </row>
@@ -6760,9 +6758,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6924,25 +6925,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57723507-2D03-46ED-A005-5642ABE4AB7F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6966,9 +6957,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57723507-2D03-46ED-A005-5642ABE4AB7F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
endring i diku.xlsx fikset matte1000
</commit_message>
<xml_diff>
--- a/Diku.xlsx
+++ b/Diku.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\OneDrive\Dokumenter\DIKU\DIKU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FFD136-909E-4859-A572-BF6F1B435114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ACA57A-D796-4845-8E9E-DA07676740B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Emner" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="vurderingskob-navn" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIKU!$C$1:$C$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIKU!$B$1:$B$43</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="607">
   <si>
     <t>institusjonsnr</t>
   </si>
@@ -1857,6 +1857,24 @@
   </si>
   <si>
     <t>Elektroteknikk og byggeautomasjon</t>
+  </si>
+  <si>
+    <t>https://student.oslomet.no/studier/-/studieinfo/emne/EMFE1000/2021/H%C3%98ST</t>
+  </si>
+  <si>
+    <t>Undervisningen organiseres i timeplanlagte arbeidsøkter. I arbeidsøktene skal studentene øve på fagstoff som blir introdusert. Innholdet i øvingene omfatter diskusjoner i grupper, individuell øving i å løse oppgaver, øvelser i problemformulering og problemløsing, og vurdering av egne og andres besvarelse av oppgaver. Studentene skal bli i stand til å vurdere egne og andres faglige arbeider, og formulere vurderinger av disse på en slik måte at vurderingen gir råd om videre studiearbeid. Øving i dette foregår i den timeplanlagte delen av arbeidsøktene. Studentene skal derfor gjennomføre ukevurderinger av oppgaver som bygger på ukeoppgaver. Informasjon om hvordan ukevurderingene skal gjennomføres, blir gitt i forelesningene.  I periodene mellom arbeidsøktene må studentene løse oppgaver. Øvingsoppgavene som blir foreslått er knyttet direkte opp mot læringsutbyttet i emnet. Egenvurdering av besvarelsene vil gi studentene innsikt i hvor stor grad målene er nådd</t>
+  </si>
+  <si>
+    <t>Individuell digital hjemmeeksamen, 5 timer.</t>
+  </si>
+  <si>
+    <t>Studenten kan: gjøre rede for den deriverte som momentan endring, ta utgangspunkt i definisjonen av den deriverte, og gjøre rede for hvordan man kan bestemme en tilnærmet verdi av den deriverte numerisk, regne ut eksakte verdier av den deriverte ved å bruke analytiske metoder, bruke den deriverte til å løse optimaliseringsproblemer, gjøre rede for det ubestemte integralet som antiderivert, bruke numeriske og analytiske metoder til å beregne bestemte integraler, forklare hvordan man kan bruke det bestemte integralet til å regne ut størrelser som f eks areal, volum, arealmomentløse systemer av differensiallikninger, ladning eller andre størrelser, gjøre rede for analytiske og numeriske løsningsmetoder av ordinære differensiallikninger, løse systemer av differensiallikninger, regne med komplekse tall, regne med vektorer, matriser og determinanter, overføre totalmatriser for lineære likningssystemer til redusert trappeform, gjøre rede for betingelser som må være oppfylt for at det skal være mulig å regne ut den inverse til matriser, gjøre rede for antall løsninger til et lineært likningssystem, beskrive lineære transformasjoner ved hjelp av matriser, bruke dataverktøy til å løse problemer i lineær algebra, løse likninger numerisk</t>
+  </si>
+  <si>
+    <t>Studenten kan: anvende den deriverte til å modellere og analysere dynamiske systemer, diskutere hvordan ideen bak definisjonen av det bestemte integralet kan brukes til å sette opp integraler for beregning av størrelser, drøfte ideene bak noen analytiske og numeriske metoder som brukes for å løse differensiallikninger, og sette opp og løse differensiallikninger for praktiske problemer som er relevante innen eget fagområde, drøfte metoder for å løse lineære likningssystemer ved hjelp av matriseregning og drøfte numeriske metoder for å løse likninger, og sette opp og løse likninger for praktiske problemer fra eget fagområde</t>
+  </si>
+  <si>
+    <t>Studenten kan: vurdere resultater fra matematiske beregninger, forklare og bruke grunnleggende numeriske algoritmer som inneholder kodeelementene tilordning, for- og while-løkker og if-tester, skrive presise forklaringer og begrunnelser til framgangsmåter, og demonstrere korrekt bruk av matematisk notasjon, vurdere egne og andre studenters faglige arbeider, og formulere skriftlige og muntlige vurderinger av disse arbeidene på en faglig korrekt og presis måte, verføre et praktisk problem fra eget fagområde til matematisk form, slik at det kan løses - analytisk eller numerisk, bruke matematiske metoder og digitale verktøy som er relevante for eget fagfelt, bruke matematikk til å kommunisere om ingeniørfaglige problemstillinger</t>
   </si>
 </sst>
 </file>
@@ -1957,7 +1975,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2000,6 +2018,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3841,8 +3862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCDD31-3723-4F19-8F81-7049F051B343}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5241,9 +5262,9 @@
         <v>455</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
-        <v>279</v>
+    <row r="28" spans="1:17" ht="263.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>601</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>114</v>
@@ -5274,22 +5295,22 @@
         <v>10</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>280</v>
+        <v>602</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>265</v>
+        <v>603</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>282</v>
+        <v>604</v>
       </c>
       <c r="P28" s="11" t="s">
-        <v>283</v>
+        <v>605</v>
       </c>
       <c r="Q28" s="11" t="s">
-        <v>284</v>
+        <v>606</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6050,7 +6071,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C43" xr:uid="{B7BCDD31-3723-4F19-8F81-7049F051B343}"/>
+  <autoFilter ref="B1:B43" xr:uid="{B7BCDD31-3723-4F19-8F81-7049F051B343}"/>
   <hyperlinks>
     <hyperlink ref="A10" r:id="rId1" xr:uid="{2D038A63-AA70-42FE-B351-24BF5DA4B8D7}"/>
     <hyperlink ref="A11" r:id="rId2" xr:uid="{75B26816-45EF-4849-B5B1-186267B860D4}"/>
@@ -6060,9 +6081,10 @@
     <hyperlink ref="A32" r:id="rId6" xr:uid="{531FA050-1969-4FF3-8924-CD48D6C2C832}"/>
     <hyperlink ref="J33" r:id="rId7" xr:uid="{C7B989CE-4C76-4DA3-8596-63088D4B5B98}"/>
     <hyperlink ref="J24" r:id="rId8" xr:uid="{6D92DA99-4575-4A19-8F85-F84B1CF8FDB6}"/>
+    <hyperlink ref="A28" r:id="rId9" xr:uid="{2B7B1F59-5D6F-4D8C-91E5-AC654BAF7199}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -6442,9 +6464,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6606,25 +6631,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57723507-2D03-46ED-A005-5642ABE4AB7F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6648,9 +6663,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57723507-2D03-46ED-A005-5642ABE4AB7F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fikset feil i excel ark
</commit_message>
<xml_diff>
--- a/Diku.xlsx
+++ b/Diku.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/rashasin_oslomet_no/Documents/Skrivebord/DIKU/DIKU-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\OneDrive\Dokumenter\DIKU\DIKU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D45DDD-6D99-4404-A6C9-D7B28C3A9329}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792AA823-F00A-4571-AD27-85DED67300EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Emner" sheetId="1" r:id="rId1"/>
@@ -1659,10 +1659,6 @@
     <t xml:space="preserve">Individuell skriftlig eksamen på 3 timer som teller 100 % </t>
   </si>
   <si>
-    <t xml:space="preserve">1) Individuell skriftlig eksamen under tilsyn på 5 timer, som teller 70 % 1) Individuell skriftlig eksamen under tilsyn på 5 timer, som teller 70 %
-</t>
-  </si>
-  <si>
     <t>Studenten: kan gjøre rede for myndighetenes krav, forskrifter, regler og bransjenormer for VVS-tekniske installasjoner, har kunnskap om energikilder og energiforsyning, har kunnskap om energi- inneklimaberegninger, har kunnskap om vannbårne oppvarmingssystemer, har kunnskap om kjølesystemer, har kunnskap ventilasjonsanlegg og ventilering av oppholdssoner, har kunnskap om sanitærtekniske installasjoner innomhus</t>
   </si>
   <si>
@@ -1869,6 +1865,10 @@
   </si>
   <si>
     <t>Studenten kan: vurdere resultater fra matematiske beregninger, forklare og bruke grunnleggende numeriske algoritmer som inneholder kodeelementene tilordning, for- og while-løkker og if-tester, skrive presise forklaringer og begrunnelser til framgangsmåter, og demonstrere korrekt bruk av matematisk notasjon, vurdere egne og andre studenters faglige arbeider, og formulere skriftlige og muntlige vurderinger av disse arbeidene på en faglig korrekt og presis måte, verføre et praktisk problem fra eget fagområde til matematisk form, slik at det kan løses - analytisk eller numerisk, bruke matematiske metoder og digitale verktøy som er relevante for eget fagfelt, bruke matematikk til å kommunisere om ingeniørfaglige problemstillinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Individuell skriftlig eksamen under tilsyn på 5 timer, som teller 70 % 2) Prosjektarbeid i gruppe som teller 30 %. Rapport vurderes.
+</t>
   </si>
 </sst>
 </file>
@@ -2018,8 +2018,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Dårlig" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperkobling" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2318,17 +2318,17 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>215</v>
       </c>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>215</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>215</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>215</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>215</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>215</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>215</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>215</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>215</v>
       </c>
@@ -2669,7 +2669,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>215</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>215</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>215</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>215</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>215</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>215</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>215</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>215</v>
       </c>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>215</v>
       </c>
@@ -2973,7 +2973,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>215</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>215</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>215</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>215</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>215</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>215</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>215</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>215</v>
       </c>
@@ -3261,7 +3261,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>215</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>215</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>215</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>215</v>
       </c>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>215</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>215</v>
       </c>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>215</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>215</v>
       </c>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>215</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>215</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>215</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>215</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>215</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>215</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>215</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>215</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>215</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>215</v>
       </c>
@@ -3856,32 +3856,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCDD31-3723-4F19-8F81-7049F051B343}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="51.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>178</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>182</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>183</v>
@@ -3931,10 +3931,10 @@
         <v>267</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="325.14999999999998" customHeight="1" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="325.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>253</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>247</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10" t="s">
@@ -3985,7 +3985,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="301.89999999999998" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="301.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>258</v>
       </c>
@@ -4009,10 +4009,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>568</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>569</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>570</v>
       </c>
       <c r="K3" s="10">
         <v>10</v>
@@ -4036,7 +4036,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>263</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="326.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="326.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>279</v>
       </c>
@@ -4111,10 +4111,10 @@
         <v>264</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>570</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>571</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>572</v>
       </c>
       <c r="K5" s="10">
         <v>10</v>
@@ -4138,7 +4138,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>285</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>247</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
@@ -4162,10 +4162,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>581</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>582</v>
       </c>
       <c r="K6" s="10">
         <v>5</v>
@@ -4189,7 +4189,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="202.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="202.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>292</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>299</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="388.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="388.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>305</v>
       </c>
@@ -4315,10 +4315,10 @@
         <v>3</v>
       </c>
       <c r="I9" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>575</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>576</v>
       </c>
       <c r="K9" s="10">
         <v>10</v>
@@ -4342,7 +4342,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>312</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="197.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>321</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="306" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="306" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>327</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>330</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P12" s="7" t="s">
         <v>331</v>
@@ -4491,7 +4491,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>333</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="191.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="191.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>342</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>360</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="95.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>367</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="147.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="147.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>403</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="216.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="216.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>404</v>
       </c>
@@ -4770,10 +4770,10 @@
         <v>5</v>
       </c>
       <c r="I18" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="J18" s="10" t="s">
         <v>591</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>592</v>
       </c>
       <c r="K18" s="10">
         <v>10</v>
@@ -4797,7 +4797,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="177.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>405</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>361</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="10" t="s">
@@ -4821,10 +4821,10 @@
         <v>5</v>
       </c>
       <c r="I19" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="J19" s="10" t="s">
         <v>577</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>578</v>
       </c>
       <c r="K19" s="10">
         <v>10</v>
@@ -4848,7 +4848,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>406</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="228.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>396</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>408</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>361</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="10" t="s">
@@ -4974,10 +4974,10 @@
         <v>5</v>
       </c>
       <c r="I22" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="J22" s="10" t="s">
         <v>579</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>580</v>
       </c>
       <c r="K22" s="10">
         <v>10</v>
@@ -5001,7 +5001,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>422</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>361</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="10" t="s">
@@ -5052,7 +5052,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>423</v>
       </c>
@@ -5076,10 +5076,10 @@
         <v>5</v>
       </c>
       <c r="I24" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="J24" s="13" t="s">
         <v>593</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>594</v>
       </c>
       <c r="K24" s="10">
         <v>10</v>
@@ -5103,7 +5103,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>432</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="305.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="305.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>439</v>
       </c>
@@ -5178,10 +5178,10 @@
         <v>6</v>
       </c>
       <c r="I26" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="J26" s="10" t="s">
         <v>583</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>584</v>
       </c>
       <c r="K26" s="10">
         <v>20</v>
@@ -5205,7 +5205,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>448</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>361</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="10" t="s">
@@ -5256,9 +5256,9 @@
         <v>453</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="263.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="263.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>114</v>
@@ -5280,34 +5280,34 @@
         <v>264</v>
       </c>
       <c r="I28" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="J28" s="10" t="s">
         <v>573</v>
       </c>
-      <c r="J28" s="10" t="s">
-        <v>574</v>
-      </c>
       <c r="K28" s="10">
         <v>10</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="M28" s="7" t="s">
         <v>307</v>
       </c>
       <c r="N28" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="O28" s="10" t="s">
         <v>601</v>
       </c>
-      <c r="O28" s="10" t="s">
+      <c r="P28" s="11" t="s">
         <v>602</v>
       </c>
-      <c r="P28" s="11" t="s">
+      <c r="Q28" s="11" t="s">
         <v>603</v>
       </c>
-      <c r="Q28" s="11" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="182.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:17" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>457</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>464</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="193.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="193.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>470</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>475</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="273.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="273.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>483</v>
       </c>
@@ -5535,10 +5535,10 @@
         <v>3</v>
       </c>
       <c r="I33" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="J33" s="13" t="s">
         <v>573</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>574</v>
       </c>
       <c r="K33" s="10">
         <v>10</v>
@@ -5562,7 +5562,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>491</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="271.89999999999998" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="271.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>499</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>147</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="K35" s="10">
         <v>10</v>
@@ -5664,7 +5664,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="211.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="211.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>509</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>505</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>247</v>
@@ -5715,7 +5715,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="260.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="260.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>516</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="154.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="154.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>522</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>529</v>
       </c>
@@ -5852,21 +5852,21 @@
         <v>533</v>
       </c>
       <c r="N39" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="O39" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="O39" s="7" t="s">
+      <c r="P39" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="P39" s="7" t="s">
+      <c r="Q39" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="Q39" s="7" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="330" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>174</v>
@@ -5891,39 +5891,39 @@
         <v>177</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="K40" s="10">
         <v>10</v>
       </c>
       <c r="L40" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="M40" s="7" t="s">
         <v>541</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>542</v>
       </c>
       <c r="N40" s="7" t="s">
         <v>275</v>
       </c>
       <c r="O40" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="P40" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="P40" s="7" t="s">
+      <c r="Q40" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="Q40" s="7" t="s">
+    </row>
+    <row r="41" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>538</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>545</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="330" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>547</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>539</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>546</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>361</v>
@@ -5939,36 +5939,36 @@
         <v>5</v>
       </c>
       <c r="I41" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="J41" s="10" t="s">
         <v>587</v>
       </c>
-      <c r="J41" s="10" t="s">
-        <v>588</v>
-      </c>
       <c r="K41" s="10">
         <v>10</v>
       </c>
       <c r="L41" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="M41" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="M41" s="7" t="s">
+      <c r="N41" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="N41" s="7" t="s">
+      <c r="O41" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="O41" s="7" t="s">
+      <c r="P41" s="7" t="s">
         <v>551</v>
       </c>
-      <c r="P41" s="7" t="s">
+      <c r="Q41" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="Q41" s="7" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="214.9" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:17" ht="214.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>131</v>
@@ -5995,27 +5995,27 @@
         <v>10</v>
       </c>
       <c r="L42" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="M42" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="M42" s="7" t="s">
+      <c r="N42" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="N42" s="7" t="s">
+      <c r="O42" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="O42" s="7" t="s">
+      <c r="P42" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="P42" s="7" t="s">
+      <c r="Q42" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="Q42" s="7" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="267.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:17" ht="267.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>163</v>
@@ -6037,31 +6037,31 @@
         <v>6</v>
       </c>
       <c r="I43" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="J43" s="10" t="s">
         <v>589</v>
-      </c>
-      <c r="J43" s="10" t="s">
-        <v>590</v>
       </c>
       <c r="K43" s="10">
         <v>20</v>
       </c>
       <c r="L43" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="M43" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="M43" s="7" t="s">
+      <c r="N43" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="N43" s="7" t="s">
+      <c r="O43" s="7" t="s">
         <v>564</v>
       </c>
-      <c r="O43" s="7" t="s">
+      <c r="P43" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="P43" s="7" t="s">
+      <c r="Q43" s="7" t="s">
         <v>566</v>
-      </c>
-      <c r="Q43" s="7" t="s">
-        <v>567</v>
       </c>
     </row>
   </sheetData>
@@ -6090,13 +6090,13 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>190</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>192</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>202</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>203</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>204</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>205</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>210</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>210</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>211</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>212</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>213</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>215</v>
       </c>
@@ -6256,7 +6256,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>217</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>219</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>220</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>221</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>223</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>226</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>227</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>229</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>231</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>234</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>235</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>236</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>237</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>238</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>239</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>240</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>244</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>246</v>
       </c>
@@ -6458,21 +6458,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E4BEBC94C57EF142B9FB66C30637CB77" ma:contentTypeVersion="6" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="7939999945ed547e26316e13f4687a8d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4987dd3-0351-42de-a520-b4ffc26db00c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a0cf29d00ec2ee5e4c529c507ebdb73" ns2:_="">
     <xsd:import namespace="a4987dd3-0351-42de-a520-b4ffc26db00c"/>
@@ -6630,10 +6615,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB936A41-5980-4213-AAA9-D29C6505E2DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a4987dd3-0351-42de-a520-b4ffc26db00c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6654,19 +6664,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB936A41-5980-4213-AAA9-D29C6505E2DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07B19B9-522F-49FB-8E18-FBE655C1A6EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a4987dd3-0351-42de-a520-b4ffc26db00c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>